<commit_message>
Update files from TestWorkbook_Excel
</commit_message>
<xml_diff>
--- a/tests/TestUtils/TestFiles/TestWorkbook_ClosedXML.xlsx
+++ b/tests/TestUtils/TestFiles/TestWorkbook_ClosedXML.xlsx
@@ -5,16 +5,16 @@
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\IO\FsSpreadsheet\tests\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\FsSpreadsheet\tests\TestUtils\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64140FFE-95F7-4477-8202-92827B72206F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B1E11E-B158-4269-8B17-EBBA9EEB720A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="0" activeTab="2" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
+    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="1" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="WithTable" sheetId="1" r:id="rId1"/>
-    <x:sheet name="Tableless" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Tableless" sheetId="4" r:id="rId2"/>
     <x:sheet name="WithTable_Duplicate" sheetId="3" r:id="rId3"/>
   </x:sheets>
   <x:definedNames/>
@@ -57,9 +57,6 @@
   </x:si>
   <x:si>
     <x:t>Hello</x:t>
-  </x:si>
-  <x:si>
-    <x:t>any</x:t>
   </x:si>
   <x:si>
     <x:t>(A) This is part 1 of 2</x:t>
@@ -120,20 +117,30 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
-    <x:cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:dxfs count="1">
+  <x:dxfs count="2">
     <x:dxf>
       <x:font>
         <x:color theme="1"/>
       </x:font>
+    </x:dxf>
+    <x:dxf>
+      <x:font>
+        <x:color theme="1"/>
+      </x:font>
+      <x:numFmt numFmtId="14" formatCode="M/d/yyyy"/>
     </x:dxf>
   </x:dxfs>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -154,7 +161,7 @@
   <x:tableColumns count="5">
     <x:tableColumn id="1" name="Numbers" dataDxfId="0"/>
     <x:tableColumn id="2" name="Strings" dataDxfId="0"/>
-    <x:tableColumn id="3" name="DateTime" dataDxfId="0"/>
+    <x:tableColumn id="3" name="DateTime" dataDxfId="1"/>
     <x:tableColumn id="4" name="ARCtrl Column" dataDxfId="0"/>
     <x:tableColumn id="5" name="ARCtrl Column " dataDxfId="0"/>
   </x:tableColumns>
@@ -168,7 +175,7 @@
   <x:tableColumns count="5">
     <x:tableColumn id="1" name="Numbers" dataDxfId="0"/>
     <x:tableColumn id="2" name="Strings" dataDxfId="0"/>
-    <x:tableColumn id="3" name="DateTime" dataDxfId="0"/>
+    <x:tableColumn id="3" name="DateTime" dataDxfId="1"/>
     <x:tableColumn id="4" name="ARCtrl Column" dataDxfId="0"/>
     <x:tableColumn id="5" name="ARCtrl Column " dataDxfId="0"/>
   </x:tableColumns>
@@ -177,7 +184,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -479,12 +486,12 @@
   <x:dimension ref="A1:E5"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="J6" sqref="J6"/>
+      <x:selection activeCell="E3" sqref="E3"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="11.420625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultColWidth="11.424911" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="2" width="11.420625" style="0" customWidth="1"/>
+    <x:col min="1" max="2" width="11.424911" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="11.710938" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="16" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="17" style="0" customWidth="1"/>
@@ -514,14 +521,14 @@
       <x:c r="B2" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="C2" s="1">
+        <x:v>45213</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -529,13 +536,13 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C3" s="1">
+        <x:v>45214</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
         <x:v>9</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -543,10 +550,10 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C4" s="1">
+        <x:v>45215</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -554,10 +561,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C5" s="1">
+        <x:v>45216</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -572,17 +579,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{2C74DDE2-CDF5-40D3-9F40-97EED0BE5279}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{A3C16715-9795-4E17-A00E-CEB100B9AE9C}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E4"/>
+  <x:dimension ref="A1:E5"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="E1" sqref="E1"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="E2" sqref="E2"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="11.420625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="2" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="10.140625" style="0" bestFit="1" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
@@ -608,14 +619,14 @@
       <x:c r="B2" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="C2" s="1">
+        <x:v>45213</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -623,13 +634,13 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C3" s="1">
+        <x:v>45214</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
         <x:v>9</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -637,15 +648,26 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C4" s="1">
+        <x:v>45215</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="0">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>6</x:v>
+      <x:c r="C5" s="1">
+        <x:v>45216</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
@@ -659,11 +681,11 @@
   </x:sheetPr>
   <x:dimension ref="B4:F8"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="K12" sqref="K12"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="I26" sqref="I26"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="11.420625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultColWidth="11.424911" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
     <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="B4" s="0" t="s">
@@ -689,14 +711,14 @@
       <x:c r="C5" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D5" s="0" t="s">
+      <x:c r="D5" s="1">
+        <x:v>45213</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="E5" s="0" t="s">
+      <x:c r="F5" s="0" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -704,13 +726,13 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D6" s="1">
+        <x:v>45214</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
         <x:v>9</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="F6" s="0" t="s">
-        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -718,10 +740,10 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D7" s="1">
+        <x:v>45215</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -729,10 +751,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D8" s="1">
+        <x:v>45216</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Add boolean column to Default TestWorkbook
</commit_message>
<xml_diff>
--- a/tests/TestUtils/TestFiles/TestWorkbook_ClosedXML.xlsx
+++ b/tests/TestUtils/TestFiles/TestWorkbook_ClosedXML.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\FsSpreadsheet\tests\TestUtils\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B1E11E-B158-4269-8B17-EBBA9EEB720A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F75E44-56D1-4133-9ACD-612009724140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="1" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="1" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="WithTable" sheetId="1" r:id="rId1"/>
@@ -48,6 +48,9 @@
   </x:si>
   <x:si>
     <x:t>DateTime</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Boolean</x:t>
   </x:si>
   <x:si>
     <x:t>ARCtrl Column</x:t>
@@ -156,28 +159,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="MyTable" displayName="MyTable" ref="A1:E5" totalsRowShown="0">
-  <x:autoFilter ref="A1:E5"/>
-  <x:tableColumns count="5">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="MyTable" displayName="MyTable" ref="A1:F5" totalsRowShown="0">
+  <x:autoFilter ref="A1:F5"/>
+  <x:tableColumns count="6">
     <x:tableColumn id="1" name="Numbers" dataDxfId="0"/>
     <x:tableColumn id="2" name="Strings" dataDxfId="0"/>
     <x:tableColumn id="3" name="DateTime" dataDxfId="1"/>
-    <x:tableColumn id="4" name="ARCtrl Column" dataDxfId="0"/>
-    <x:tableColumn id="5" name="ARCtrl Column " dataDxfId="0"/>
+    <x:tableColumn id="4" name="Boolean" dataDxfId="1"/>
+    <x:tableColumn id="5" name="ARCtrl Column" dataDxfId="0"/>
+    <x:tableColumn id="6" name="ARCtrl Column " dataDxfId="0"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="MyOtherTable" displayName="MyOtherTable" ref="B4:F8" totalsRowShown="0">
-  <x:autoFilter ref="B4:F8"/>
-  <x:tableColumns count="5">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="MyOtherTable" displayName="MyOtherTable" ref="B4:G8" totalsRowShown="0">
+  <x:autoFilter ref="B4:G8"/>
+  <x:tableColumns count="6">
     <x:tableColumn id="1" name="Numbers" dataDxfId="0"/>
     <x:tableColumn id="2" name="Strings" dataDxfId="0"/>
     <x:tableColumn id="3" name="DateTime" dataDxfId="1"/>
-    <x:tableColumn id="4" name="ARCtrl Column" dataDxfId="0"/>
-    <x:tableColumn id="5" name="ARCtrl Column " dataDxfId="0"/>
+    <x:tableColumn id="4" name="Boolean" dataDxfId="1"/>
+    <x:tableColumn id="5" name="ARCtrl Column" dataDxfId="0"/>
+    <x:tableColumn id="6" name="ARCtrl Column " dataDxfId="0"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -483,10 +488,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E5"/>
+  <x:dimension ref="A1:F5"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="E3" sqref="E3"/>
+      <x:selection activeCell="F5" sqref="F5 A1:F5"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="11.424911" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +502,7 @@
     <x:col min="5" max="5" width="17" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -513,58 +518,73 @@
       <x:c r="E1" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C2" s="1">
         <x:v>45213</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>6</x:v>
+      <x:c r="D2" s="1" t="b">
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="F2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A3" s="0">
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C3" s="1">
         <x:v>45214</x:v>
       </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="D3" s="1" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A4" s="0">
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C4" s="1">
         <x:v>45215</x:v>
       </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="D4" s="1" t="b">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A5" s="0">
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C5" s="1">
         <x:v>45216</x:v>
+      </x:c>
+      <x:c r="D5" s="1" t="b">
+        <x:v>0</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -583,19 +603,19 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E5"/>
+  <x:dimension ref="A1:F5"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="E2" sqref="E2"/>
+      <x:selection activeCell="D6" sqref="D6"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="2" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="10.140625" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="4" width="10.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -611,58 +631,73 @@
       <x:c r="E1" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C2" s="1">
         <x:v>45213</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>6</x:v>
+      <x:c r="D2" s="1" t="b">
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="F2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A3" s="0">
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C3" s="1">
         <x:v>45214</x:v>
       </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="D3" s="1" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A4" s="0">
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C4" s="1">
         <x:v>45215</x:v>
       </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="D4" s="1" t="b">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A5" s="0">
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C5" s="1">
         <x:v>45216</x:v>
+      </x:c>
+      <x:c r="D5" s="1" t="b">
+        <x:v>0</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -679,15 +714,15 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="B4:F8"/>
+  <x:dimension ref="B4:G8"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="I26" sqref="I26"/>
+      <x:selection activeCell="F7" sqref="F7"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="11.424911" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
-    <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <x:row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="B4" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -703,58 +738,73 @@
       <x:c r="F4" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="G4" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="B5" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D5" s="1">
         <x:v>45213</x:v>
       </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>6</x:v>
+      <x:c r="E5" s="1" t="b">
+        <x:v>1</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="G5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="B6" s="0">
         <x:v>2</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D6" s="1">
         <x:v>45214</x:v>
       </x:c>
-      <x:c r="F6" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="E6" s="1" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="B7" s="0">
         <x:v>3</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D7" s="1">
         <x:v>45215</x:v>
       </x:c>
-    </x:row>
-    <x:row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="E7" s="1" t="b">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="B8" s="0">
         <x:v>4</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D8" s="1">
         <x:v>45216</x:v>
+      </x:c>
+      <x:c r="E8" s="1" t="b">
+        <x:v>0</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Add FsSpreadsheet tests and update testFile to include Time in DateTime
</commit_message>
<xml_diff>
--- a/tests/TestUtils/TestFiles/TestWorkbook_ClosedXML.xlsx
+++ b/tests/TestUtils/TestFiles/TestWorkbook_ClosedXML.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\FsSpreadsheet\tests\TestUtils\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F75E44-56D1-4133-9ACD-612009724140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D519B4-9EB9-4270-AC51-4E9C555EC60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="1" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="WithTable" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
+    <x:numFmt numFmtId="165" formatCode="d/m/yy\ h:mm;@"/>
   </x:numFmts>
   <x:fonts count="2" x14ac:knownFonts="1">
     <x:font>
@@ -120,15 +120,19 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
+  <x:cellStyleXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,7 +168,7 @@
   <x:tableColumns count="6">
     <x:tableColumn id="1" name="Numbers" dataDxfId="0"/>
     <x:tableColumn id="2" name="Strings" dataDxfId="0"/>
-    <x:tableColumn id="3" name="DateTime" dataDxfId="1"/>
+    <x:tableColumn id="3" name="DateTime"/>
     <x:tableColumn id="4" name="Boolean" dataDxfId="1"/>
     <x:tableColumn id="5" name="ARCtrl Column" dataDxfId="0"/>
     <x:tableColumn id="6" name="ARCtrl Column " dataDxfId="0"/>
@@ -490,14 +494,14 @@
   </x:sheetPr>
   <x:dimension ref="A1:F5"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="F5" sqref="F5 A1:F5"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="E11" sqref="E11"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="11.424911" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="2" width="11.424911" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="11.710938" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="25.855469" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="16" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="17" style="0" customWidth="1"/>
   </x:cols>
@@ -549,8 +553,8 @@
       <x:c r="B3" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="C3" s="1">
-        <x:v>45214</x:v>
+      <x:c r="C3" s="2">
+        <x:v>45214.75</x:v>
       </x:c>
       <x:c r="D3" s="1" t="b">
         <x:v>0</x:v>
@@ -566,8 +570,8 @@
       <x:c r="B4" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="C4" s="1">
-        <x:v>45215</x:v>
+      <x:c r="C4" s="2">
+        <x:v>45215.8333333333</x:v>
       </x:c>
       <x:c r="D4" s="1" t="b">
         <x:v>1</x:v>
@@ -605,8 +609,8 @@
   </x:sheetPr>
   <x:dimension ref="A1:F5"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="D6" sqref="D6"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="F1" sqref="F1"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix DateTime format :bug:
</commit_message>
<xml_diff>
--- a/tests/TestUtils/TestFiles/TestWorkbook_ClosedXML.xlsx
+++ b/tests/TestUtils/TestFiles/TestWorkbook_ClosedXML.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\FsSpreadsheet\tests\TestUtils\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343F6A22-0824-4E43-AE04-176496A6F8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE64C58-D250-4F5C-9030-D8C8F36DA3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="2" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="1" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="WithTable" sheetId="1" r:id="rId1"/>
@@ -609,14 +609,15 @@
   </x:sheetPr>
   <x:dimension ref="A1:F5"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="F1" sqref="F1"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="C3" sqref="C3 C3:C4"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="2" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="3" max="4" width="10.140625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="13.285156" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="10.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -666,8 +667,8 @@
       <x:c r="B3" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="C3" s="1">
-        <x:v>45214</x:v>
+      <x:c r="C3" s="2">
+        <x:v>45214.75</x:v>
       </x:c>
       <x:c r="D3" s="1" t="b">
         <x:v>0</x:v>
@@ -683,8 +684,8 @@
       <x:c r="B4" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="C4" s="1">
-        <x:v>45215</x:v>
+      <x:c r="C4" s="2">
+        <x:v>45215.8333333333</x:v>
       </x:c>
       <x:c r="D4" s="1" t="b">
         <x:v>1</x:v>
@@ -720,7 +721,7 @@
   </x:sheetPr>
   <x:dimension ref="B4:G8"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
+    <x:sheetView workbookViewId="0">
       <x:selection activeCell="G12" sqref="G12"/>
     </x:sheetView>
   </x:sheetViews>

</xml_diff>

<commit_message>
fix libre file parsing and update test files
</commit_message>
<xml_diff>
--- a/tests/TestUtils/TestFiles/TestWorkbook_ClosedXML.xlsx
+++ b/tests/TestUtils/TestFiles/TestWorkbook_ClosedXML.xlsx
@@ -5,12 +5,12 @@
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\FsSpreadsheet\tests\TestUtils\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\IO\FsSpreadsheet\tests\TestUtils\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE64C58-D250-4F5C-9030-D8C8F36DA3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01576CE0-678A-4608-B9EF-37C8B90F67AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="1" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="0" activeTab="2" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="WithTable" sheetId="1" r:id="rId1"/>
@@ -129,25 +129,20 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="3">
+  <x:cellXfs count="4">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <x:cellStyle name="Standard" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:dxfs count="2">
+  <x:dxfs count="1">
     <x:dxf>
       <x:font>
         <x:color theme="1"/>
       </x:font>
-    </x:dxf>
-    <x:dxf>
-      <x:font>
-        <x:color theme="1"/>
-      </x:font>
-      <x:numFmt numFmtId="14" formatCode="M/d/yyyy"/>
     </x:dxf>
   </x:dxfs>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -169,7 +164,7 @@
     <x:tableColumn id="1" name="Numbers" dataDxfId="0"/>
     <x:tableColumn id="2" name="Strings" dataDxfId="0"/>
     <x:tableColumn id="3" name="DateTime"/>
-    <x:tableColumn id="4" name="Boolean" dataDxfId="1"/>
+    <x:tableColumn id="4" name="Boolean" dataDxfId="0"/>
     <x:tableColumn id="5" name="ARCtrl Column" dataDxfId="0"/>
     <x:tableColumn id="6" name="ARCtrl Column " dataDxfId="0"/>
   </x:tableColumns>
@@ -184,7 +179,7 @@
     <x:tableColumn id="1" name="Numbers" dataDxfId="0"/>
     <x:tableColumn id="2" name="Strings" dataDxfId="0"/>
     <x:tableColumn id="3" name="DateTime"/>
-    <x:tableColumn id="4" name="Boolean" dataDxfId="1"/>
+    <x:tableColumn id="4" name="Boolean" dataDxfId="0"/>
     <x:tableColumn id="5" name="ARCtrl Column" dataDxfId="0"/>
     <x:tableColumn id="6" name="ARCtrl Column " dataDxfId="0"/>
   </x:tableColumns>
@@ -193,7 +188,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -495,10 +490,10 @@
   <x:dimension ref="A1:F5"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="C3" sqref="C3"/>
+      <x:selection activeCell="E23" sqref="E23"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="11.424911" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="11.424911" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="2" width="11.424911" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="25.855469" style="0" customWidth="1"/>
@@ -536,7 +531,7 @@
       <x:c r="C2" s="1">
         <x:v>45213</x:v>
       </x:c>
-      <x:c r="D2" s="1" t="b">
+      <x:c r="D2" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
@@ -556,7 +551,7 @@
       <x:c r="C3" s="2">
         <x:v>45214.75</x:v>
       </x:c>
-      <x:c r="D3" s="1" t="b">
+      <x:c r="D3" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
@@ -573,7 +568,7 @@
       <x:c r="C4" s="2">
         <x:v>45215.8333333333</x:v>
       </x:c>
-      <x:c r="D4" s="1" t="b">
+      <x:c r="D4" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
     </x:row>
@@ -587,7 +582,7 @@
       <x:c r="C5" s="1">
         <x:v>45216</x:v>
       </x:c>
-      <x:c r="D5" s="1" t="b">
+      <x:c r="D5" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
     </x:row>
@@ -609,13 +604,13 @@
   </x:sheetPr>
   <x:dimension ref="A1:F5"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="C3" sqref="C3 C3:C4"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="I19" sqref="I19"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="9.139196" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="2" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="1" max="2" width="9.139196" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="13.285156" style="0" bestFit="1" customWidth="1"/>
     <x:col min="4" max="4" width="10.140625" style="0" customWidth="1"/>
   </x:cols>
@@ -650,7 +645,7 @@
       <x:c r="C2" s="1">
         <x:v>45213</x:v>
       </x:c>
-      <x:c r="D2" s="1" t="b">
+      <x:c r="D2" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
@@ -670,7 +665,7 @@
       <x:c r="C3" s="2">
         <x:v>45214.75</x:v>
       </x:c>
-      <x:c r="D3" s="1" t="b">
+      <x:c r="D3" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
@@ -687,7 +682,7 @@
       <x:c r="C4" s="2">
         <x:v>45215.8333333333</x:v>
       </x:c>
-      <x:c r="D4" s="1" t="b">
+      <x:c r="D4" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
     </x:row>
@@ -701,7 +696,7 @@
       <x:c r="C5" s="1">
         <x:v>45216</x:v>
       </x:c>
-      <x:c r="D5" s="1" t="b">
+      <x:c r="D5" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
     </x:row>
@@ -721,11 +716,11 @@
   </x:sheetPr>
   <x:dimension ref="B4:G8"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="G12" sqref="G12"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="M11" sqref="M11"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="11.424911" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="11.424911" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="3" width="11.424911" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="13.285156" style="0" bestFit="1" customWidth="1"/>
@@ -761,7 +756,7 @@
       <x:c r="D5" s="1">
         <x:v>45213</x:v>
       </x:c>
-      <x:c r="E5" s="1" t="b">
+      <x:c r="E5" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
@@ -781,7 +776,7 @@
       <x:c r="D6" s="2">
         <x:v>45214.75</x:v>
       </x:c>
-      <x:c r="E6" s="1" t="b">
+      <x:c r="E6" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
@@ -798,7 +793,7 @@
       <x:c r="D7" s="2">
         <x:v>45215.8333333333</x:v>
       </x:c>
-      <x:c r="E7" s="1" t="b">
+      <x:c r="E7" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
     </x:row>
@@ -812,7 +807,7 @@
       <x:c r="D8" s="1">
         <x:v>45216</x:v>
       </x:c>
-      <x:c r="E8" s="1" t="b">
+      <x:c r="E8" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Fix ExcelIO: bool & float write. Fix exceljs: table postion write, cell value type read and write, confusing naming. Add scripts for fsspreadsheet write. :sparkles:🤡
</commit_message>
<xml_diff>
--- a/tests/TestUtils/TestFiles/TestWorkbook_ClosedXML.xlsx
+++ b/tests/TestUtils/TestFiles/TestWorkbook_ClosedXML.xlsx
@@ -5,12 +5,12 @@
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\IO\FsSpreadsheet\tests\TestUtils\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\FsSpreadsheet\tests\TestUtils\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01576CE0-678A-4608-B9EF-37C8B90F67AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D9724B-E1DD-4CE8-B902-5C9BA3C810AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="0" activeTab="2" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="1" xr2:uid="{D39F27F7-D601-47AA-88F1-83333031ED1D}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="WithTable" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="3">
+  <x:cellStyleXfs count="4">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -128,15 +128,18 @@
     <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
   <x:cellXfs count="4">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <x:xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
-    <x:cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
   <x:dxfs count="1">
     <x:dxf>
@@ -161,7 +164,7 @@
 <x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="MyTable" displayName="MyTable" ref="A1:F5" totalsRowShown="0">
   <x:autoFilter ref="A1:F5"/>
   <x:tableColumns count="6">
-    <x:tableColumn id="1" name="Numbers" dataDxfId="0"/>
+    <x:tableColumn id="1" name="Numbers"/>
     <x:tableColumn id="2" name="Strings" dataDxfId="0"/>
     <x:tableColumn id="3" name="DateTime"/>
     <x:tableColumn id="4" name="Boolean" dataDxfId="0"/>
@@ -176,7 +179,7 @@
 <x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="MyOtherTable" displayName="MyOtherTable" ref="B4:G8" totalsRowShown="0">
   <x:autoFilter ref="B4:G8"/>
   <x:tableColumns count="6">
-    <x:tableColumn id="1" name="Numbers" dataDxfId="0"/>
+    <x:tableColumn id="1" name="Numbers"/>
     <x:tableColumn id="2" name="Strings" dataDxfId="0"/>
     <x:tableColumn id="3" name="DateTime"/>
     <x:tableColumn id="4" name="Boolean" dataDxfId="0"/>
@@ -188,7 +191,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -490,10 +493,10 @@
   <x:dimension ref="A1:F5"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="E23" sqref="E23"/>
+      <x:selection activeCell="A5" sqref="A5"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="11.424911" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultColWidth="11.424911" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="2" width="11.424911" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="25.855469" style="0" customWidth="1"/>
@@ -573,8 +576,8 @@
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="0">
-        <x:v>4</x:v>
+      <x:c r="A5" s="3">
+        <x:v>4.269</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
         <x:v>12</x:v>
@@ -604,11 +607,11 @@
   </x:sheetPr>
   <x:dimension ref="A1:F5"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="I19" sqref="I19"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A5" sqref="A5"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="9.139196" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultColWidth="9.139196" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="2" width="9.139196" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="13.285156" style="0" bestFit="1" customWidth="1"/>
@@ -687,8 +690,8 @@
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="0">
-        <x:v>4</x:v>
+      <x:c r="A5" s="3">
+        <x:v>4.269</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
         <x:v>12</x:v>
@@ -716,11 +719,11 @@
   </x:sheetPr>
   <x:dimension ref="B4:G8"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="M11" sqref="M11"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="B8" sqref="B8"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="11.424911" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultColWidth="11.424911" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="3" width="11.424911" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="13.285156" style="0" bestFit="1" customWidth="1"/>
@@ -798,8 +801,8 @@
       </x:c>
     </x:row>
     <x:row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <x:c r="B8" s="0">
-        <x:v>4</x:v>
+      <x:c r="B8" s="3">
+        <x:v>4.269</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
         <x:v>12</x:v>

</xml_diff>